<commit_message>
negative sales bug fixed
</commit_message>
<xml_diff>
--- a/ClinicaReportes/resources/Felix Ortega Dongo30888.xlsx
+++ b/ClinicaReportes/resources/Felix Ortega Dongo30888.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="70">
   <si>
     <t>CMP</t>
   </si>
@@ -266,7 +266,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:O59"/>
+  <dimension ref="B2:O116"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -280,6 +280,10 @@
     <col min="7" max="7" width="10.30078125" customWidth="true" bestFit="true"/>
     <col min="8" max="8" width="14.484375" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="9.32421875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="8.48046875" customWidth="true" bestFit="true"/>
+    <col min="12" max="12" width="9.40625" customWidth="true" bestFit="true"/>
+    <col min="13" max="13" width="8.48046875" customWidth="true" bestFit="true"/>
+    <col min="14" max="14" width="8.578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="2">
@@ -378,13 +382,13 @@
         <v>21</v>
       </c>
       <c r="K4" t="n">
-        <v>247.02</v>
+        <v>-247.02</v>
       </c>
       <c r="L4" t="n">
         <v>11.12</v>
       </c>
       <c r="M4" t="n">
-        <v>235.9</v>
+        <v>-258.14</v>
       </c>
     </row>
     <row r="5">
@@ -2278,8 +2282,2003 @@
       </c>
     </row>
     <row r="59">
-      <c r="N59" t="n">
-        <v>2752.100000000002</v>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>13</v>
+      </c>
+      <c r="H59" t="s">
+        <v>14</v>
+      </c>
+      <c r="I59" t="s">
+        <v>15</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L59" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="s">
+        <v>16</v>
+      </c>
+      <c r="D60" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60" t="s">
+        <v>19</v>
+      </c>
+      <c r="H60" t="s">
+        <v>20</v>
+      </c>
+      <c r="I60" t="s">
+        <v>21</v>
+      </c>
+      <c r="K60" t="n">
+        <v>-247.02</v>
+      </c>
+      <c r="L60" t="n">
+        <v>11.12</v>
+      </c>
+      <c r="M60" t="n">
+        <v>-258.14</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="s">
+        <v>16</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G61" t="s">
+        <v>19</v>
+      </c>
+      <c r="H61" t="s">
+        <v>20</v>
+      </c>
+      <c r="I61" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" t="n">
+        <v>247.02</v>
+      </c>
+      <c r="L61" t="n">
+        <v>11.12</v>
+      </c>
+      <c r="M61" t="n">
+        <v>235.9</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="C62" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" t="s">
+        <v>23</v>
+      </c>
+      <c r="E62" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" t="s">
+        <v>18</v>
+      </c>
+      <c r="G62" t="s">
+        <v>13</v>
+      </c>
+      <c r="H62" t="s">
+        <v>24</v>
+      </c>
+      <c r="I62" t="s">
+        <v>21</v>
+      </c>
+      <c r="K62" t="n">
+        <v>267.62</v>
+      </c>
+      <c r="L62" t="n">
+        <v>12.04</v>
+      </c>
+      <c r="M62" t="n">
+        <v>255.58</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" t="s">
+        <v>19</v>
+      </c>
+      <c r="H63" t="s">
+        <v>20</v>
+      </c>
+      <c r="I63" t="s">
+        <v>26</v>
+      </c>
+      <c r="K63" t="n">
+        <v>52.92</v>
+      </c>
+      <c r="L63" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="M63" t="n">
+        <v>50.54</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" t="s">
+        <v>19</v>
+      </c>
+      <c r="H64" t="s">
+        <v>20</v>
+      </c>
+      <c r="I64" t="s">
+        <v>27</v>
+      </c>
+      <c r="K64" t="n">
+        <v>21.17</v>
+      </c>
+      <c r="L64" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M64" t="n">
+        <v>20.22</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" t="s">
+        <v>19</v>
+      </c>
+      <c r="H65" t="s">
+        <v>20</v>
+      </c>
+      <c r="I65" t="s">
+        <v>28</v>
+      </c>
+      <c r="K65" t="n">
+        <v>21.17</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M65" t="n">
+        <v>20.22</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" t="s">
+        <v>25</v>
+      </c>
+      <c r="D66" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" t="s">
+        <v>29</v>
+      </c>
+      <c r="F66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" t="s">
+        <v>19</v>
+      </c>
+      <c r="H66" t="s">
+        <v>20</v>
+      </c>
+      <c r="I66" t="s">
+        <v>30</v>
+      </c>
+      <c r="K66" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="L66" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M66" t="n">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" t="s">
+        <v>25</v>
+      </c>
+      <c r="D67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" t="s">
+        <v>19</v>
+      </c>
+      <c r="H67" t="s">
+        <v>20</v>
+      </c>
+      <c r="I67" t="s">
+        <v>31</v>
+      </c>
+      <c r="K67" t="n">
+        <v>42.34</v>
+      </c>
+      <c r="L67" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="M67" t="n">
+        <v>40.43</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" t="s">
+        <v>25</v>
+      </c>
+      <c r="D68" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68" t="s">
+        <v>29</v>
+      </c>
+      <c r="F68" t="s">
+        <v>18</v>
+      </c>
+      <c r="G68" t="s">
+        <v>19</v>
+      </c>
+      <c r="H68" t="s">
+        <v>33</v>
+      </c>
+      <c r="I68" t="s">
+        <v>30</v>
+      </c>
+      <c r="K68" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="L68" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M68" t="n">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>25</v>
+      </c>
+      <c r="D69" t="s">
+        <v>32</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>18</v>
+      </c>
+      <c r="G69" t="s">
+        <v>19</v>
+      </c>
+      <c r="H69" t="s">
+        <v>33</v>
+      </c>
+      <c r="I69" t="s">
+        <v>28</v>
+      </c>
+      <c r="K69" t="n">
+        <v>21.17</v>
+      </c>
+      <c r="L69" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M69" t="n">
+        <v>20.22</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C70" t="s">
+        <v>25</v>
+      </c>
+      <c r="D70" t="s">
+        <v>32</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" t="s">
+        <v>18</v>
+      </c>
+      <c r="G70" t="s">
+        <v>19</v>
+      </c>
+      <c r="H70" t="s">
+        <v>33</v>
+      </c>
+      <c r="I70" t="s">
+        <v>34</v>
+      </c>
+      <c r="K70" t="n">
+        <v>19.42</v>
+      </c>
+      <c r="L70" t="n">
+        <v>0.87</v>
+      </c>
+      <c r="M70" t="n">
+        <v>18.55</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="C71" t="s">
+        <v>35</v>
+      </c>
+      <c r="D71" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" t="s">
+        <v>29</v>
+      </c>
+      <c r="F71" t="s">
+        <v>37</v>
+      </c>
+      <c r="G71" t="s">
+        <v>19</v>
+      </c>
+      <c r="H71" t="s">
+        <v>38</v>
+      </c>
+      <c r="I71" t="s">
+        <v>30</v>
+      </c>
+      <c r="K71" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L71" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M71" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C72" t="s">
+        <v>35</v>
+      </c>
+      <c r="D72" t="s">
+        <v>36</v>
+      </c>
+      <c r="E72" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" t="s">
+        <v>37</v>
+      </c>
+      <c r="G72" t="s">
+        <v>19</v>
+      </c>
+      <c r="H72" t="s">
+        <v>38</v>
+      </c>
+      <c r="I72" t="s">
+        <v>21</v>
+      </c>
+      <c r="K72" t="n">
+        <v>267.62</v>
+      </c>
+      <c r="L72" t="n">
+        <v>12.04</v>
+      </c>
+      <c r="M72" t="n">
+        <v>255.58</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="C73" t="s">
+        <v>35</v>
+      </c>
+      <c r="D73" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" t="s">
+        <v>37</v>
+      </c>
+      <c r="G73" t="s">
+        <v>19</v>
+      </c>
+      <c r="H73" t="s">
+        <v>38</v>
+      </c>
+      <c r="I73" t="s">
+        <v>26</v>
+      </c>
+      <c r="K73" t="n">
+        <v>57.33</v>
+      </c>
+      <c r="L73" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="M73" t="n">
+        <v>54.75</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="C74" t="s">
+        <v>35</v>
+      </c>
+      <c r="D74" t="s">
+        <v>39</v>
+      </c>
+      <c r="E74" t="s">
+        <v>29</v>
+      </c>
+      <c r="F74" t="s">
+        <v>37</v>
+      </c>
+      <c r="G74" t="s">
+        <v>40</v>
+      </c>
+      <c r="H74" t="s">
+        <v>41</v>
+      </c>
+      <c r="I74" t="s">
+        <v>42</v>
+      </c>
+      <c r="K74" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L74" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M74" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" t="s">
+        <v>43</v>
+      </c>
+      <c r="E75" t="s">
+        <v>29</v>
+      </c>
+      <c r="F75" t="s">
+        <v>37</v>
+      </c>
+      <c r="G75" t="s">
+        <v>19</v>
+      </c>
+      <c r="H75" t="s">
+        <v>44</v>
+      </c>
+      <c r="I75" t="s">
+        <v>30</v>
+      </c>
+      <c r="K75" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L75" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M75" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="C76" t="s">
+        <v>35</v>
+      </c>
+      <c r="D76" t="s">
+        <v>43</v>
+      </c>
+      <c r="E76" t="s">
+        <v>11</v>
+      </c>
+      <c r="F76" t="s">
+        <v>37</v>
+      </c>
+      <c r="G76" t="s">
+        <v>19</v>
+      </c>
+      <c r="H76" t="s">
+        <v>44</v>
+      </c>
+      <c r="I76" t="s">
+        <v>28</v>
+      </c>
+      <c r="K76" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L76" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M76" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="C77" t="s">
+        <v>35</v>
+      </c>
+      <c r="D77" t="s">
+        <v>43</v>
+      </c>
+      <c r="E77" t="s">
+        <v>11</v>
+      </c>
+      <c r="F77" t="s">
+        <v>37</v>
+      </c>
+      <c r="G77" t="s">
+        <v>19</v>
+      </c>
+      <c r="H77" t="s">
+        <v>44</v>
+      </c>
+      <c r="I77" t="s">
+        <v>27</v>
+      </c>
+      <c r="K77" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L77" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M77" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" t="s">
+        <v>35</v>
+      </c>
+      <c r="D78" t="s">
+        <v>43</v>
+      </c>
+      <c r="E78" t="s">
+        <v>11</v>
+      </c>
+      <c r="F78" t="s">
+        <v>37</v>
+      </c>
+      <c r="G78" t="s">
+        <v>19</v>
+      </c>
+      <c r="H78" t="s">
+        <v>44</v>
+      </c>
+      <c r="I78" t="s">
+        <v>45</v>
+      </c>
+      <c r="K78" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L78" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M78" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79" t="s">
+        <v>43</v>
+      </c>
+      <c r="E79" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" t="s">
+        <v>37</v>
+      </c>
+      <c r="G79" t="s">
+        <v>19</v>
+      </c>
+      <c r="H79" t="s">
+        <v>44</v>
+      </c>
+      <c r="I79" t="s">
+        <v>46</v>
+      </c>
+      <c r="K79" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L79" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M79" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" t="s">
+        <v>47</v>
+      </c>
+      <c r="D80" t="s">
+        <v>39</v>
+      </c>
+      <c r="E80" t="s">
+        <v>29</v>
+      </c>
+      <c r="F80" t="s">
+        <v>37</v>
+      </c>
+      <c r="G80" t="s">
+        <v>19</v>
+      </c>
+      <c r="H80" t="s">
+        <v>41</v>
+      </c>
+      <c r="I80" t="s">
+        <v>30</v>
+      </c>
+      <c r="K80" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L80" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M80" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" t="s">
+        <v>48</v>
+      </c>
+      <c r="E81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" t="s">
+        <v>37</v>
+      </c>
+      <c r="G81" t="s">
+        <v>19</v>
+      </c>
+      <c r="H81" t="s">
+        <v>49</v>
+      </c>
+      <c r="I81" t="s">
+        <v>34</v>
+      </c>
+      <c r="K81" t="n">
+        <v>21.04</v>
+      </c>
+      <c r="L81" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M81" t="n">
+        <v>20.09</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" t="s">
+        <v>48</v>
+      </c>
+      <c r="E82" t="s">
+        <v>29</v>
+      </c>
+      <c r="F82" t="s">
+        <v>37</v>
+      </c>
+      <c r="G82" t="s">
+        <v>19</v>
+      </c>
+      <c r="H82" t="s">
+        <v>49</v>
+      </c>
+      <c r="I82" t="s">
+        <v>30</v>
+      </c>
+      <c r="K82" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L82" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M82" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="C83" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" t="s">
+        <v>50</v>
+      </c>
+      <c r="E83" t="s">
+        <v>29</v>
+      </c>
+      <c r="F83" t="s">
+        <v>37</v>
+      </c>
+      <c r="G83" t="s">
+        <v>19</v>
+      </c>
+      <c r="H83" t="s">
+        <v>51</v>
+      </c>
+      <c r="I83" t="s">
+        <v>30</v>
+      </c>
+      <c r="K83" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L83" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M83" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="C84" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" t="s">
+        <v>50</v>
+      </c>
+      <c r="E84" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" t="s">
+        <v>37</v>
+      </c>
+      <c r="G84" t="s">
+        <v>19</v>
+      </c>
+      <c r="H84" t="s">
+        <v>51</v>
+      </c>
+      <c r="I84" t="s">
+        <v>34</v>
+      </c>
+      <c r="K84" t="n">
+        <v>21.04</v>
+      </c>
+      <c r="L84" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M84" t="n">
+        <v>20.09</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="C85" t="s">
+        <v>47</v>
+      </c>
+      <c r="D85" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" t="s">
+        <v>37</v>
+      </c>
+      <c r="G85" t="s">
+        <v>19</v>
+      </c>
+      <c r="H85" t="s">
+        <v>51</v>
+      </c>
+      <c r="I85" t="s">
+        <v>21</v>
+      </c>
+      <c r="K85" t="n">
+        <v>267.62</v>
+      </c>
+      <c r="L85" t="n">
+        <v>12.04</v>
+      </c>
+      <c r="M85" t="n">
+        <v>255.58</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C86" t="s">
+        <v>47</v>
+      </c>
+      <c r="D86" t="s">
+        <v>50</v>
+      </c>
+      <c r="E86" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" t="s">
+        <v>37</v>
+      </c>
+      <c r="G86" t="s">
+        <v>19</v>
+      </c>
+      <c r="H86" t="s">
+        <v>51</v>
+      </c>
+      <c r="I86" t="s">
+        <v>46</v>
+      </c>
+      <c r="K86" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L86" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M86" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="C87" t="s">
+        <v>47</v>
+      </c>
+      <c r="D87" t="s">
+        <v>50</v>
+      </c>
+      <c r="E87" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" t="s">
+        <v>37</v>
+      </c>
+      <c r="G87" t="s">
+        <v>19</v>
+      </c>
+      <c r="H87" t="s">
+        <v>51</v>
+      </c>
+      <c r="I87" t="s">
+        <v>45</v>
+      </c>
+      <c r="K87" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L87" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M87" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="C88" t="s">
+        <v>47</v>
+      </c>
+      <c r="D88" t="s">
+        <v>50</v>
+      </c>
+      <c r="E88" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" t="s">
+        <v>37</v>
+      </c>
+      <c r="G88" t="s">
+        <v>19</v>
+      </c>
+      <c r="H88" t="s">
+        <v>51</v>
+      </c>
+      <c r="I88" t="s">
+        <v>27</v>
+      </c>
+      <c r="K88" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L88" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M88" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="C89" t="s">
+        <v>47</v>
+      </c>
+      <c r="D89" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" t="s">
+        <v>37</v>
+      </c>
+      <c r="G89" t="s">
+        <v>19</v>
+      </c>
+      <c r="H89" t="s">
+        <v>51</v>
+      </c>
+      <c r="I89" t="s">
+        <v>28</v>
+      </c>
+      <c r="K89" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L89" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M89" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="C90" t="s">
+        <v>47</v>
+      </c>
+      <c r="D90" t="s">
+        <v>52</v>
+      </c>
+      <c r="E90" t="s">
+        <v>29</v>
+      </c>
+      <c r="F90" t="s">
+        <v>37</v>
+      </c>
+      <c r="G90" t="s">
+        <v>19</v>
+      </c>
+      <c r="H90" t="s">
+        <v>53</v>
+      </c>
+      <c r="I90" t="s">
+        <v>30</v>
+      </c>
+      <c r="K90" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L90" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M90" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="s">
+        <v>8</v>
+      </c>
+      <c r="C91" t="s">
+        <v>47</v>
+      </c>
+      <c r="D91" t="s">
+        <v>52</v>
+      </c>
+      <c r="E91" t="s">
+        <v>11</v>
+      </c>
+      <c r="F91" t="s">
+        <v>37</v>
+      </c>
+      <c r="G91" t="s">
+        <v>19</v>
+      </c>
+      <c r="H91" t="s">
+        <v>53</v>
+      </c>
+      <c r="I91" t="s">
+        <v>45</v>
+      </c>
+      <c r="K91" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L91" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M91" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="C92" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" t="s">
+        <v>52</v>
+      </c>
+      <c r="E92" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" t="s">
+        <v>37</v>
+      </c>
+      <c r="G92" t="s">
+        <v>19</v>
+      </c>
+      <c r="H92" t="s">
+        <v>53</v>
+      </c>
+      <c r="I92" t="s">
+        <v>34</v>
+      </c>
+      <c r="K92" t="n">
+        <v>21.04</v>
+      </c>
+      <c r="L92" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M92" t="n">
+        <v>20.09</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="s">
+        <v>8</v>
+      </c>
+      <c r="C93" t="s">
+        <v>47</v>
+      </c>
+      <c r="D93" t="s">
+        <v>52</v>
+      </c>
+      <c r="E93" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" t="s">
+        <v>37</v>
+      </c>
+      <c r="G93" t="s">
+        <v>19</v>
+      </c>
+      <c r="H93" t="s">
+        <v>53</v>
+      </c>
+      <c r="I93" t="s">
+        <v>28</v>
+      </c>
+      <c r="K93" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L93" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M93" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s">
+        <v>8</v>
+      </c>
+      <c r="C94" t="s">
+        <v>47</v>
+      </c>
+      <c r="D94" t="s">
+        <v>54</v>
+      </c>
+      <c r="E94" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" t="s">
+        <v>37</v>
+      </c>
+      <c r="G94" t="s">
+        <v>19</v>
+      </c>
+      <c r="H94" t="s">
+        <v>55</v>
+      </c>
+      <c r="I94" t="s">
+        <v>45</v>
+      </c>
+      <c r="K94" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L94" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M94" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="s">
+        <v>8</v>
+      </c>
+      <c r="C95" t="s">
+        <v>47</v>
+      </c>
+      <c r="D95" t="s">
+        <v>54</v>
+      </c>
+      <c r="E95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" t="s">
+        <v>37</v>
+      </c>
+      <c r="G95" t="s">
+        <v>19</v>
+      </c>
+      <c r="H95" t="s">
+        <v>55</v>
+      </c>
+      <c r="I95" t="s">
+        <v>27</v>
+      </c>
+      <c r="K95" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L95" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M95" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="s">
+        <v>8</v>
+      </c>
+      <c r="C96" t="s">
+        <v>47</v>
+      </c>
+      <c r="D96" t="s">
+        <v>54</v>
+      </c>
+      <c r="E96" t="s">
+        <v>29</v>
+      </c>
+      <c r="F96" t="s">
+        <v>37</v>
+      </c>
+      <c r="G96" t="s">
+        <v>19</v>
+      </c>
+      <c r="H96" t="s">
+        <v>55</v>
+      </c>
+      <c r="I96" t="s">
+        <v>30</v>
+      </c>
+      <c r="K96" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L96" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M96" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>47</v>
+      </c>
+      <c r="D97" t="s">
+        <v>54</v>
+      </c>
+      <c r="E97" t="s">
+        <v>11</v>
+      </c>
+      <c r="F97" t="s">
+        <v>37</v>
+      </c>
+      <c r="G97" t="s">
+        <v>19</v>
+      </c>
+      <c r="H97" t="s">
+        <v>55</v>
+      </c>
+      <c r="I97" t="s">
+        <v>28</v>
+      </c>
+      <c r="K97" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L97" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M97" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="s">
+        <v>8</v>
+      </c>
+      <c r="C98" t="s">
+        <v>56</v>
+      </c>
+      <c r="D98" t="s">
+        <v>57</v>
+      </c>
+      <c r="E98" t="s">
+        <v>29</v>
+      </c>
+      <c r="F98" t="s">
+        <v>37</v>
+      </c>
+      <c r="G98" t="s">
+        <v>19</v>
+      </c>
+      <c r="H98" t="s">
+        <v>58</v>
+      </c>
+      <c r="I98" t="s">
+        <v>30</v>
+      </c>
+      <c r="K98" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L98" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M98" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="s">
+        <v>8</v>
+      </c>
+      <c r="C99" t="s">
+        <v>56</v>
+      </c>
+      <c r="D99" t="s">
+        <v>57</v>
+      </c>
+      <c r="E99" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" t="s">
+        <v>37</v>
+      </c>
+      <c r="G99" t="s">
+        <v>19</v>
+      </c>
+      <c r="H99" t="s">
+        <v>58</v>
+      </c>
+      <c r="I99" t="s">
+        <v>45</v>
+      </c>
+      <c r="K99" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L99" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M99" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="s">
+        <v>8</v>
+      </c>
+      <c r="C100" t="s">
+        <v>56</v>
+      </c>
+      <c r="D100" t="s">
+        <v>57</v>
+      </c>
+      <c r="E100" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100" t="s">
+        <v>37</v>
+      </c>
+      <c r="G100" t="s">
+        <v>19</v>
+      </c>
+      <c r="H100" t="s">
+        <v>58</v>
+      </c>
+      <c r="I100" t="s">
+        <v>34</v>
+      </c>
+      <c r="K100" t="n">
+        <v>21.04</v>
+      </c>
+      <c r="L100" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M100" t="n">
+        <v>20.09</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="s">
+        <v>8</v>
+      </c>
+      <c r="C101" t="s">
+        <v>56</v>
+      </c>
+      <c r="D101" t="s">
+        <v>57</v>
+      </c>
+      <c r="E101" t="s">
+        <v>11</v>
+      </c>
+      <c r="F101" t="s">
+        <v>37</v>
+      </c>
+      <c r="G101" t="s">
+        <v>19</v>
+      </c>
+      <c r="H101" t="s">
+        <v>58</v>
+      </c>
+      <c r="I101" t="s">
+        <v>28</v>
+      </c>
+      <c r="K101" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L101" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M101" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="s">
+        <v>8</v>
+      </c>
+      <c r="C102" t="s">
+        <v>56</v>
+      </c>
+      <c r="D102" t="s">
+        <v>59</v>
+      </c>
+      <c r="E102" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" t="s">
+        <v>37</v>
+      </c>
+      <c r="G102" t="s">
+        <v>19</v>
+      </c>
+      <c r="H102" t="s">
+        <v>60</v>
+      </c>
+      <c r="I102" t="s">
+        <v>27</v>
+      </c>
+      <c r="K102" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L102" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M102" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" t="s">
+        <v>56</v>
+      </c>
+      <c r="D103" t="s">
+        <v>59</v>
+      </c>
+      <c r="E103" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" t="s">
+        <v>37</v>
+      </c>
+      <c r="G103" t="s">
+        <v>19</v>
+      </c>
+      <c r="H103" t="s">
+        <v>60</v>
+      </c>
+      <c r="I103" t="s">
+        <v>28</v>
+      </c>
+      <c r="K103" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L103" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M103" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" t="s">
+        <v>56</v>
+      </c>
+      <c r="D104" t="s">
+        <v>59</v>
+      </c>
+      <c r="E104" t="s">
+        <v>11</v>
+      </c>
+      <c r="F104" t="s">
+        <v>37</v>
+      </c>
+      <c r="G104" t="s">
+        <v>19</v>
+      </c>
+      <c r="H104" t="s">
+        <v>60</v>
+      </c>
+      <c r="I104" t="s">
+        <v>34</v>
+      </c>
+      <c r="K104" t="n">
+        <v>21.04</v>
+      </c>
+      <c r="L104" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M104" t="n">
+        <v>20.09</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105" t="s">
+        <v>56</v>
+      </c>
+      <c r="D105" t="s">
+        <v>59</v>
+      </c>
+      <c r="E105" t="s">
+        <v>29</v>
+      </c>
+      <c r="F105" t="s">
+        <v>37</v>
+      </c>
+      <c r="G105" t="s">
+        <v>19</v>
+      </c>
+      <c r="H105" t="s">
+        <v>60</v>
+      </c>
+      <c r="I105" t="s">
+        <v>30</v>
+      </c>
+      <c r="K105" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L105" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M105" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" t="s">
+        <v>8</v>
+      </c>
+      <c r="C106" t="s">
+        <v>56</v>
+      </c>
+      <c r="D106" t="s">
+        <v>61</v>
+      </c>
+      <c r="E106" t="s">
+        <v>11</v>
+      </c>
+      <c r="F106" t="s">
+        <v>37</v>
+      </c>
+      <c r="G106" t="s">
+        <v>19</v>
+      </c>
+      <c r="H106" t="s">
+        <v>62</v>
+      </c>
+      <c r="I106" t="s">
+        <v>27</v>
+      </c>
+      <c r="K106" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L106" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M106" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" t="s">
+        <v>8</v>
+      </c>
+      <c r="C107" t="s">
+        <v>56</v>
+      </c>
+      <c r="D107" t="s">
+        <v>61</v>
+      </c>
+      <c r="E107" t="s">
+        <v>11</v>
+      </c>
+      <c r="F107" t="s">
+        <v>37</v>
+      </c>
+      <c r="G107" t="s">
+        <v>19</v>
+      </c>
+      <c r="H107" t="s">
+        <v>62</v>
+      </c>
+      <c r="I107" t="s">
+        <v>34</v>
+      </c>
+      <c r="K107" t="n">
+        <v>21.04</v>
+      </c>
+      <c r="L107" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="M107" t="n">
+        <v>20.09</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" t="s">
+        <v>8</v>
+      </c>
+      <c r="C108" t="s">
+        <v>56</v>
+      </c>
+      <c r="D108" t="s">
+        <v>61</v>
+      </c>
+      <c r="E108" t="s">
+        <v>29</v>
+      </c>
+      <c r="F108" t="s">
+        <v>37</v>
+      </c>
+      <c r="G108" t="s">
+        <v>19</v>
+      </c>
+      <c r="H108" t="s">
+        <v>62</v>
+      </c>
+      <c r="I108" t="s">
+        <v>30</v>
+      </c>
+      <c r="K108" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="L108" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M108" t="n">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" t="s">
+        <v>8</v>
+      </c>
+      <c r="C109" t="s">
+        <v>56</v>
+      </c>
+      <c r="D109" t="s">
+        <v>61</v>
+      </c>
+      <c r="E109" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" t="s">
+        <v>37</v>
+      </c>
+      <c r="G109" t="s">
+        <v>19</v>
+      </c>
+      <c r="H109" t="s">
+        <v>62</v>
+      </c>
+      <c r="I109" t="s">
+        <v>28</v>
+      </c>
+      <c r="K109" t="n">
+        <v>22.93</v>
+      </c>
+      <c r="L109" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="M109" t="n">
+        <v>21.9</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" t="s">
+        <v>8</v>
+      </c>
+      <c r="C110" t="s">
+        <v>63</v>
+      </c>
+      <c r="D110" t="s">
+        <v>64</v>
+      </c>
+      <c r="E110" t="s">
+        <v>29</v>
+      </c>
+      <c r="F110" t="s">
+        <v>65</v>
+      </c>
+      <c r="G110" t="s">
+        <v>19</v>
+      </c>
+      <c r="H110" t="s">
+        <v>66</v>
+      </c>
+      <c r="I110" t="s">
+        <v>30</v>
+      </c>
+      <c r="K110" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="L110" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M110" t="n">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" t="s">
+        <v>8</v>
+      </c>
+      <c r="C111" t="s">
+        <v>63</v>
+      </c>
+      <c r="D111" t="s">
+        <v>64</v>
+      </c>
+      <c r="E111" t="s">
+        <v>11</v>
+      </c>
+      <c r="F111" t="s">
+        <v>65</v>
+      </c>
+      <c r="G111" t="s">
+        <v>19</v>
+      </c>
+      <c r="H111" t="s">
+        <v>66</v>
+      </c>
+      <c r="I111" t="s">
+        <v>26</v>
+      </c>
+      <c r="K111" t="n">
+        <v>51.82</v>
+      </c>
+      <c r="L111" t="n">
+        <v>2.33</v>
+      </c>
+      <c r="M111" t="n">
+        <v>49.49</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" t="s">
+        <v>8</v>
+      </c>
+      <c r="C112" t="s">
+        <v>63</v>
+      </c>
+      <c r="D112" t="s">
+        <v>64</v>
+      </c>
+      <c r="E112" t="s">
+        <v>11</v>
+      </c>
+      <c r="F112" t="s">
+        <v>65</v>
+      </c>
+      <c r="G112" t="s">
+        <v>19</v>
+      </c>
+      <c r="H112" t="s">
+        <v>66</v>
+      </c>
+      <c r="I112" t="s">
+        <v>21</v>
+      </c>
+      <c r="K112" t="n">
+        <v>241.88</v>
+      </c>
+      <c r="L112" t="n">
+        <v>10.88</v>
+      </c>
+      <c r="M112" t="n">
+        <v>231.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" t="s">
+        <v>8</v>
+      </c>
+      <c r="C113" t="s">
+        <v>63</v>
+      </c>
+      <c r="D113" t="s">
+        <v>64</v>
+      </c>
+      <c r="E113" t="s">
+        <v>11</v>
+      </c>
+      <c r="F113" t="s">
+        <v>65</v>
+      </c>
+      <c r="G113" t="s">
+        <v>19</v>
+      </c>
+      <c r="H113" t="s">
+        <v>66</v>
+      </c>
+      <c r="I113" t="s">
+        <v>45</v>
+      </c>
+      <c r="K113" t="n">
+        <v>20.73</v>
+      </c>
+      <c r="L113" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="M113" t="n">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" t="s">
+        <v>8</v>
+      </c>
+      <c r="C114" t="s">
+        <v>63</v>
+      </c>
+      <c r="D114" t="s">
+        <v>64</v>
+      </c>
+      <c r="E114" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" t="s">
+        <v>65</v>
+      </c>
+      <c r="G114" t="s">
+        <v>19</v>
+      </c>
+      <c r="H114" t="s">
+        <v>66</v>
+      </c>
+      <c r="I114" t="s">
+        <v>27</v>
+      </c>
+      <c r="K114" t="n">
+        <v>20.73</v>
+      </c>
+      <c r="L114" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="M114" t="n">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="B115" t="s">
+        <v>8</v>
+      </c>
+      <c r="C115" t="s">
+        <v>63</v>
+      </c>
+      <c r="D115" t="s">
+        <v>64</v>
+      </c>
+      <c r="E115" t="s">
+        <v>11</v>
+      </c>
+      <c r="F115" t="s">
+        <v>65</v>
+      </c>
+      <c r="G115" t="s">
+        <v>19</v>
+      </c>
+      <c r="H115" t="s">
+        <v>66</v>
+      </c>
+      <c r="I115" t="s">
+        <v>28</v>
+      </c>
+      <c r="K115" t="n">
+        <v>20.73</v>
+      </c>
+      <c r="L115" t="n">
+        <v>0.93</v>
+      </c>
+      <c r="M115" t="n">
+        <v>19.8</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="N116" t="n">
+        <v>4752.020000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>